<commit_message>
Enhance sentiment analysis functionality: add fallback mechanisms for news retrieval, update sentiment results, and include requirements for new libraries.
</commit_message>
<xml_diff>
--- a/aspect_sentiment_results.xlsx
+++ b/aspect_sentiment_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>headline</t>
   </si>
@@ -28,37 +28,40 @@
     <t>score</t>
   </si>
   <si>
-    <t>Tata Motors reports record profits for Q1</t>
-  </si>
-  <si>
-    <t>New electric vehicle lineup unveiled by Tata Motors</t>
-  </si>
-  <si>
-    <t>Strong sales boost Tata Motors’ revenue</t>
-  </si>
-  <si>
-    <t>Tata Motors invests in EV battery production</t>
+    <t>Tata Motors Likely To Launch Iveco Products In India, Other Markets - NDTV Profit</t>
+  </si>
+  <si>
+    <t>Tata Motors To Raise Over Rs 10,000 Crore In 18 Months To Acquire Iveco - NDTV Profit</t>
+  </si>
+  <si>
+    <t>Head: “Logical next step”: India’s Tata Motors to buy Italy’s Iveco for €3.6bn - Global Construction Review</t>
+  </si>
+  <si>
+    <t>Tata Motors seeks to expand revenues, access new technologies with $4.5 bln Iveco deal - The Economic Times</t>
+  </si>
+  <si>
+    <t>Will Tata Motors Slip Below ₹600? Deven Choksey On $4B Iveco Deal - Business Today</t>
+  </si>
+  <si>
+    <t>Tata revs up the global game. How Iveco fits in - The Economic Times</t>
+  </si>
+  <si>
+    <t>Tata Motors Share Price Rebounds On Inveco Acquisition For Rs 33,360 crore - NDTV Profit</t>
+  </si>
+  <si>
+    <t>Tata Harrier EV deliveries begin: Range, features, price and more - The Times of India</t>
+  </si>
+  <si>
+    <t>Tata Harrier.ev Deliveries Begin In India: Range, Price, Specs, Features, And More - NDTV</t>
   </si>
   <si>
     <t>profit</t>
   </si>
   <si>
-    <t>electric vehicle</t>
-  </si>
-  <si>
-    <t>sales</t>
-  </si>
-  <si>
     <t>EV</t>
   </si>
   <si>
-    <t>revenue</t>
-  </si>
-  <si>
-    <t>LABEL_2</t>
-  </si>
-  <si>
-    <t>LABEL_1</t>
+    <t>Neutral</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,13 +444,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>0.7311153411865234</v>
+        <v>0.9149685502052307</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -455,13 +458,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>0.7282027006149292</v>
+        <v>0.9274094700813293</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -469,55 +472,97 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>0.6263706088066101</v>
+        <v>0.9292269945144653</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>0.6263706088066101</v>
+        <v>0.6270380616188049</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>0.6263706088066101</v>
+        <v>0.8742959499359131</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0.8027606606483459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0.9321960806846619</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="D7">
-        <v>0.753658652305603</v>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0.8456907868385315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0.8990907073020935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>